<commit_message>
Verifica degli headers dei fogli su datasource con quelli di input
</commit_message>
<xml_diff>
--- a/Solution/FilesEditor.Tests/TestFiles/InputFiles/Budget.xlsx
+++ b/Solution/FilesEditor.Tests/TestFiles/InputFiles/Budget.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fperrino\Desktop\KPI UT_LAVORO_LEFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\FilesEditor.Tests\TestFiles\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4BA2E7-622D-4B45-BA3F-52FE297613BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C4C6508F-7D0B-44EB-BB17-EA1BBBA9CD16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
   <si>
     <t>da considerare?_</t>
   </si>
@@ -177,13 +176,40 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Business TMP</t>
+  </si>
+  <si>
+    <t>CATEGORIA</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>totale Gamberini</t>
+  </si>
+  <si>
+    <t>INT2</t>
+  </si>
+  <si>
+    <t>EST3</t>
+  </si>
+  <si>
+    <t>totale Lanzarini</t>
+  </si>
+  <si>
+    <t>TOTALE TOT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,8 +217,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,8 +246,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -214,15 +260,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Accent5" xfId="1" builtinId="45"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -554,19 +628,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B6B056-DB09-4CC0-8666-36FBC99AE47C}">
-  <dimension ref="A2:AE4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AN4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="AF2" sqref="AF2:AN2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" ht="15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,8 +735,35 @@
       <c r="AE2" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="AF2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -753,7 +855,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40">
       <c r="A4" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
Migliorie interfaccia e messaggi
</commit_message>
<xml_diff>
--- a/Solution/FilesEditor.Tests/TestFiles/InputFiles/Budget.xlsx
+++ b/Solution/FilesEditor.Tests/TestFiles/InputFiles/Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\FilesEditor.Tests\TestFiles\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01EC746-70C0-4612-AEF1-EE27BADFE6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7D86BB-F407-40A6-A3DD-DC0799160538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="72">
   <si>
     <t>da considerare?_</t>
   </si>
@@ -230,31 +230,28 @@
     <t>Pluto</t>
   </si>
   <si>
-    <t>abcde</t>
-  </si>
-  <si>
-    <t>abcd qualsiasi cosa</t>
-  </si>
-  <si>
-    <t>mikecccc</t>
-  </si>
-  <si>
-    <t>cosa cccc</t>
-  </si>
-  <si>
-    <t>a*cccc</t>
-  </si>
-  <si>
-    <t>bb anything bb</t>
-  </si>
-  <si>
-    <t>aaaappppp</t>
-  </si>
-  <si>
-    <t>aaaailmn</t>
-  </si>
-  <si>
-    <t>efmikegh</t>
+    <t>Caso D</t>
+  </si>
+  <si>
+    <t>Caso 1</t>
+  </si>
+  <si>
+    <t>Pippo 1</t>
+  </si>
+  <si>
+    <t>Pippo 2</t>
+  </si>
+  <si>
+    <t>Pippo 3</t>
+  </si>
+  <si>
+    <t>Pluto 1</t>
+  </si>
+  <si>
+    <t>Pluto 2</t>
+  </si>
+  <si>
+    <t>Pluto 3</t>
   </si>
 </sst>
 </file>
@@ -683,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AN26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG26" sqref="AG13:AG26"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AG23" sqref="AG23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,10 +913,10 @@
         <v>35</v>
       </c>
       <c r="AF3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG3" t="s">
         <v>56</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>64</v>
       </c>
       <c r="AH3">
         <v>1</v>
@@ -1041,10 +1038,10 @@
         <v>35</v>
       </c>
       <c r="AF4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG4" t="s">
         <v>57</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>72</v>
       </c>
       <c r="AH4">
         <f t="shared" ref="AH4:AN5" si="1">AH3+10</f>
@@ -1167,10 +1164,10 @@
         <v>35</v>
       </c>
       <c r="AF5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AG5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="AH5">
         <f t="shared" si="1"/>
@@ -1293,10 +1290,10 @@
         <v>35</v>
       </c>
       <c r="AF6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="AG6" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="AH6">
         <f t="shared" ref="AH6:AN6" si="2">AH5+10</f>
@@ -1419,10 +1416,10 @@
         <v>35</v>
       </c>
       <c r="AF7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AG7" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="AH7">
         <f t="shared" ref="AH7:AN7" si="3">AH6+10</f>
@@ -1545,10 +1542,10 @@
         <v>35</v>
       </c>
       <c r="AF8" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="AG8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="AH8">
         <f t="shared" ref="AH8:AN8" si="4">AH7+10</f>
@@ -1671,10 +1668,10 @@
         <v>35</v>
       </c>
       <c r="AF9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AG9" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="AH9">
         <f t="shared" ref="AH9:AN9" si="5">AH8+10</f>
@@ -1797,10 +1794,10 @@
         <v>35</v>
       </c>
       <c r="AF10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="AG10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="AH10">
         <f t="shared" ref="AH10:AN10" si="6">AH9+10</f>
@@ -1923,10 +1920,10 @@
         <v>35</v>
       </c>
       <c r="AF11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AG11" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="AH11">
         <f t="shared" ref="AH11:AN11" si="7">AH10+10</f>
@@ -2049,10 +2046,10 @@
         <v>35</v>
       </c>
       <c r="AF12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="AG12" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="AH12">
         <f t="shared" ref="AH12:AN12" si="8">AH11+10</f>
@@ -2175,10 +2172,10 @@
         <v>35</v>
       </c>
       <c r="AF13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="AG13" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="AH13">
         <f t="shared" ref="AH13:AN13" si="9">AH12+10</f>
@@ -2301,10 +2298,10 @@
         <v>35</v>
       </c>
       <c r="AF14" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="AG14" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="AH14">
         <f t="shared" ref="AH14:AN14" si="10">AH13+10</f>
@@ -2427,10 +2424,10 @@
         <v>35</v>
       </c>
       <c r="AF15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AG15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="AH15">
         <f t="shared" ref="AH15:AN15" si="11">AH14+10</f>
@@ -2553,10 +2550,10 @@
         <v>35</v>
       </c>
       <c r="AF16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="AG16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AH16">
         <f t="shared" ref="AH16:AN16" si="12">AH15+10</f>
@@ -2679,10 +2676,10 @@
         <v>35</v>
       </c>
       <c r="AF17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AG17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH17">
         <f t="shared" ref="AH17:AN17" si="13">AH16+10</f>
@@ -2805,10 +2802,10 @@
         <v>35</v>
       </c>
       <c r="AF18" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="AG18" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="AH18">
         <f t="shared" ref="AH18:AN18" si="14">AH17+10</f>
@@ -2931,10 +2928,10 @@
         <v>35</v>
       </c>
       <c r="AF19" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="AG19" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="AH19">
         <f t="shared" ref="AH19:AN19" si="15">AH18+10</f>
@@ -3057,10 +3054,10 @@
         <v>35</v>
       </c>
       <c r="AF20" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="AG20" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="AH20">
         <f t="shared" ref="AH20:AN20" si="16">AH19+10</f>
@@ -3183,10 +3180,10 @@
         <v>35</v>
       </c>
       <c r="AF21" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="AG21" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="AH21">
         <f t="shared" ref="AH21:AN21" si="17">AH20+10</f>
@@ -3309,10 +3306,10 @@
         <v>35</v>
       </c>
       <c r="AF22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AG22" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="AH22">
         <f t="shared" ref="AH22:AN22" si="18">AH21+10</f>
@@ -3435,10 +3432,10 @@
         <v>35</v>
       </c>
       <c r="AF23" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AG23" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="AH23">
         <f t="shared" ref="AH23:AN23" si="19">AH22+10</f>
@@ -3561,10 +3558,10 @@
         <v>35</v>
       </c>
       <c r="AF24" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="AG24" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="AH24">
         <f t="shared" ref="AH24:AN24" si="20">AH23+10</f>

</xml_diff>

<commit_message>
Logica di append per superdettagli
</commit_message>
<xml_diff>
--- a/Solution/FilesEditor.Tests/TestFiles/InputFiles/Budget.xlsx
+++ b/Solution/FilesEditor.Tests/TestFiles/InputFiles/Budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\FilesEditor.Tests\TestFiles\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7D86BB-F407-40A6-A3DD-DC0799160538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC992F96-A794-4321-A91B-8AFF6F7ED35D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -680,9 +680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AN26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AG23" sqref="AG23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1044,11 +1042,10 @@
         <v>57</v>
       </c>
       <c r="AH4">
-        <f t="shared" ref="AH4:AN5" si="1">AH3+10</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="AI4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AH4:AN5" si="1">AI3+10</f>
         <v>12</v>
       </c>
       <c r="AJ4">
@@ -1170,8 +1167,7 @@
         <v>64</v>
       </c>
       <c r="AH5">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="AI5">
         <f t="shared" si="1"/>
@@ -1296,11 +1292,10 @@
         <v>65</v>
       </c>
       <c r="AH6">
-        <f t="shared" ref="AH6:AN6" si="2">AH5+10</f>
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="AI6">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AH6:AN6" si="2">AI5+10</f>
         <v>32</v>
       </c>
       <c r="AJ6">
@@ -1422,11 +1417,10 @@
         <v>61</v>
       </c>
       <c r="AH7">
-        <f t="shared" ref="AH7:AN7" si="3">AH6+10</f>
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="AI7">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AH7:AN7" si="3">AI6+10</f>
         <v>42</v>
       </c>
       <c r="AJ7">
@@ -1548,11 +1542,10 @@
         <v>60</v>
       </c>
       <c r="AH8">
-        <f t="shared" ref="AH8:AN8" si="4">AH7+10</f>
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="AI8">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AH8:AN8" si="4">AI7+10</f>
         <v>52</v>
       </c>
       <c r="AJ8">
@@ -1674,11 +1667,10 @@
         <v>58</v>
       </c>
       <c r="AH9">
-        <f t="shared" ref="AH9:AN9" si="5">AH8+10</f>
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="AI9">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="AH9:AN9" si="5">AI8+10</f>
         <v>62</v>
       </c>
       <c r="AJ9">
@@ -1800,11 +1792,10 @@
         <v>62</v>
       </c>
       <c r="AH10">
-        <f t="shared" ref="AH10:AN10" si="6">AH9+10</f>
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="AI10">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="AH10:AN10" si="6">AI9+10</f>
         <v>72</v>
       </c>
       <c r="AJ10">
@@ -1926,11 +1917,10 @@
         <v>56</v>
       </c>
       <c r="AH11">
-        <f t="shared" ref="AH11:AN11" si="7">AH10+10</f>
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="AI11">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="AH11:AN11" si="7">AI10+10</f>
         <v>82</v>
       </c>
       <c r="AJ11">
@@ -2052,11 +2042,10 @@
         <v>57</v>
       </c>
       <c r="AH12">
-        <f t="shared" ref="AH12:AN12" si="8">AH11+10</f>
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="AI12">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="AH12:AN12" si="8">AI11+10</f>
         <v>92</v>
       </c>
       <c r="AJ12">
@@ -2178,11 +2167,10 @@
         <v>64</v>
       </c>
       <c r="AH13">
-        <f t="shared" ref="AH13:AN13" si="9">AH12+10</f>
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="AI13">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="AH13:AN13" si="9">AI12+10</f>
         <v>102</v>
       </c>
       <c r="AJ13">
@@ -2304,11 +2292,10 @@
         <v>65</v>
       </c>
       <c r="AH14">
-        <f t="shared" ref="AH14:AN14" si="10">AH13+10</f>
-        <v>111</v>
+        <v>12</v>
       </c>
       <c r="AI14">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="AH14:AN14" si="10">AI13+10</f>
         <v>112</v>
       </c>
       <c r="AJ14">
@@ -2430,11 +2417,10 @@
         <v>61</v>
       </c>
       <c r="AH15">
-        <f t="shared" ref="AH15:AN15" si="11">AH14+10</f>
-        <v>121</v>
+        <v>13</v>
       </c>
       <c r="AI15">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="AH15:AN15" si="11">AI14+10</f>
         <v>122</v>
       </c>
       <c r="AJ15">
@@ -2556,11 +2542,10 @@
         <v>60</v>
       </c>
       <c r="AH16">
-        <f t="shared" ref="AH16:AN16" si="12">AH15+10</f>
-        <v>131</v>
+        <v>14</v>
       </c>
       <c r="AI16">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="AH16:AN16" si="12">AI15+10</f>
         <v>132</v>
       </c>
       <c r="AJ16">
@@ -2682,11 +2667,10 @@
         <v>58</v>
       </c>
       <c r="AH17">
-        <f t="shared" ref="AH17:AN17" si="13">AH16+10</f>
-        <v>141</v>
+        <v>15</v>
       </c>
       <c r="AI17">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="AH17:AN17" si="13">AI16+10</f>
         <v>142</v>
       </c>
       <c r="AJ17">
@@ -2808,11 +2792,10 @@
         <v>62</v>
       </c>
       <c r="AH18">
-        <f t="shared" ref="AH18:AN18" si="14">AH17+10</f>
-        <v>151</v>
+        <v>16</v>
       </c>
       <c r="AI18">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="AH18:AN18" si="14">AI17+10</f>
         <v>152</v>
       </c>
       <c r="AJ18">
@@ -2934,11 +2917,10 @@
         <v>66</v>
       </c>
       <c r="AH19">
-        <f t="shared" ref="AH19:AN19" si="15">AH18+10</f>
-        <v>161</v>
+        <v>17</v>
       </c>
       <c r="AI19">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="AH19:AN19" si="15">AI18+10</f>
         <v>162</v>
       </c>
       <c r="AJ19">
@@ -3060,11 +3042,10 @@
         <v>67</v>
       </c>
       <c r="AH20">
-        <f t="shared" ref="AH20:AN20" si="16">AH19+10</f>
-        <v>171</v>
+        <v>18</v>
       </c>
       <c r="AI20">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="AH20:AN20" si="16">AI19+10</f>
         <v>172</v>
       </c>
       <c r="AJ20">
@@ -3186,11 +3167,10 @@
         <v>68</v>
       </c>
       <c r="AH21">
-        <f t="shared" ref="AH21:AN21" si="17">AH20+10</f>
-        <v>181</v>
+        <v>19</v>
       </c>
       <c r="AI21">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="AH21:AN21" si="17">AI20+10</f>
         <v>182</v>
       </c>
       <c r="AJ21">
@@ -3312,11 +3292,10 @@
         <v>69</v>
       </c>
       <c r="AH22">
-        <f t="shared" ref="AH22:AN22" si="18">AH21+10</f>
-        <v>191</v>
+        <v>20</v>
       </c>
       <c r="AI22">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="AH22:AN22" si="18">AI21+10</f>
         <v>192</v>
       </c>
       <c r="AJ22">
@@ -3438,11 +3417,10 @@
         <v>70</v>
       </c>
       <c r="AH23">
-        <f t="shared" ref="AH23:AN23" si="19">AH22+10</f>
-        <v>201</v>
+        <v>21</v>
       </c>
       <c r="AI23">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="AH23:AN23" si="19">AI22+10</f>
         <v>202</v>
       </c>
       <c r="AJ23">
@@ -3564,11 +3542,10 @@
         <v>71</v>
       </c>
       <c r="AH24">
-        <f t="shared" ref="AH24:AN24" si="20">AH23+10</f>
-        <v>211</v>
+        <v>22</v>
       </c>
       <c r="AI24">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="AH24:AN24" si="20">AI23+10</f>
         <v>212</v>
       </c>
       <c r="AJ24">
@@ -3690,11 +3667,10 @@
         <v>59</v>
       </c>
       <c r="AH25">
-        <f t="shared" ref="AH25:AN25" si="21">AH24+10</f>
-        <v>221</v>
+        <v>23</v>
       </c>
       <c r="AI25">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="AH25:AN25" si="21">AI24+10</f>
         <v>222</v>
       </c>
       <c r="AJ25">
@@ -3816,11 +3792,10 @@
         <v>59</v>
       </c>
       <c r="AH26">
-        <f t="shared" ref="AH26:AN26" si="22">AH25+10</f>
-        <v>231</v>
+        <v>24</v>
       </c>
       <c r="AI26">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="AH26:AN26" si="22">AI25+10</f>
         <v>232</v>
       </c>
       <c r="AJ26">

</xml_diff>